<commit_message>
PAS-9757: TECH DEBT - Cleanup related to removal of STAT/Choice Tier from VIN Upload
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_CA_CHOICE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Desktop\SUITE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSAA\CODE\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="63">
   <si>
     <t>VIN</t>
   </si>
@@ -173,24 +173,12 @@
     <t>RESTRAINTS_DISCOUNT</t>
   </si>
   <si>
-    <t>K</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>TEST</t>
   </si>
   <si>
-    <t>STAT</t>
-  </si>
-  <si>
-    <t>CHOICE_TIER</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -207,9 +195,6 @@
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
   <si>
     <t>invalidVin</t>
@@ -571,37 +556,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL6"/>
+  <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AC1" activeCellId="1" sqref="Z1:Z6 AC1:AC6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" customWidth="1"/>
-    <col min="21" max="21" width="22.85546875" customWidth="1"/>
-    <col min="23" max="23" width="22.28515625" customWidth="1"/>
-    <col min="24" max="24" width="20.85546875" customWidth="1"/>
-    <col min="25" max="25" width="34.7109375" customWidth="1"/>
-    <col min="26" max="26" width="6.5703125" customWidth="1"/>
-    <col min="27" max="27" width="14.85546875" customWidth="1"/>
-    <col min="28" max="29" width="16.28515625" customWidth="1"/>
-    <col min="35" max="35" width="15.140625" customWidth="1"/>
-    <col min="37" max="37" width="22.7109375" customWidth="1"/>
-    <col min="38" max="38" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" customWidth="1"/>
+    <col min="21" max="21" width="22.88671875" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" customWidth="1"/>
+    <col min="24" max="24" width="20.88671875" customWidth="1"/>
+    <col min="25" max="25" width="34.6640625" customWidth="1"/>
+    <col min="26" max="26" width="14.88671875" customWidth="1"/>
+    <col min="27" max="27" width="16.33203125" customWidth="1"/>
+    <col min="33" max="33" width="15.109375" customWidth="1"/>
+    <col min="35" max="35" width="22.6640625" customWidth="1"/>
+    <col min="36" max="36" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,60 +662,54 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AL1" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C2" s="3">
         <v>2018</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
@@ -746,13 +724,13 @@
         <v>29</v>
       </c>
       <c r="J2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>29</v>
@@ -793,64 +771,58 @@
       <c r="Y2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="3" t="s">
-        <v>54</v>
+      <c r="Z2" s="3">
+        <v>39</v>
       </c>
       <c r="AA2" s="3">
         <v>39</v>
       </c>
-      <c r="AB2" s="3">
-        <v>39</v>
+      <c r="AB2" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="AC2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG2">
+        <v>20010101</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>49</v>
       </c>
-      <c r="AD2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI2">
-        <v>20010101</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
         <v>57</v>
-      </c>
-      <c r="F3" t="s">
-        <v>62</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>28</v>
@@ -862,13 +834,13 @@
         <v>29</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>29</v>
@@ -909,64 +881,58 @@
       <c r="Y3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z3" s="3" t="s">
-        <v>54</v>
+      <c r="Z3" s="3">
+        <v>39</v>
       </c>
       <c r="AA3" s="3">
         <v>39</v>
       </c>
-      <c r="AB3" s="3">
-        <v>39</v>
+      <c r="AB3" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="AC3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG3">
+        <v>20000101</v>
+      </c>
+      <c r="AH3" t="s">
         <v>49</v>
       </c>
-      <c r="AD3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AF3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI3">
-        <v>20000101</v>
+      <c r="AI3" t="s">
+        <v>38</v>
       </c>
       <c r="AJ3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C4" s="3">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>28</v>
@@ -978,13 +944,13 @@
         <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>29</v>
@@ -1025,64 +991,58 @@
       <c r="Y4" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z4" s="3" t="s">
-        <v>54</v>
+      <c r="Z4" s="3">
+        <v>39</v>
       </c>
       <c r="AA4" s="3">
         <v>39</v>
       </c>
-      <c r="AB4" s="3">
-        <v>39</v>
+      <c r="AB4" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="AC4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG4">
+        <v>20150101</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ4" t="s">
         <v>49</v>
       </c>
-      <c r="AD4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI4">
-        <v>20150101</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C5" s="3">
         <v>2018</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>28</v>
@@ -1094,13 +1054,13 @@
         <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>29</v>
@@ -1141,61 +1101,55 @@
       <c r="Y5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z5" s="3" t="s">
-        <v>61</v>
+      <c r="Z5" s="3">
+        <v>39</v>
       </c>
       <c r="AA5" s="3">
         <v>39</v>
       </c>
-      <c r="AB5" s="3">
-        <v>39</v>
+      <c r="AB5" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="AC5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG5">
+        <v>20190101</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ5" t="s">
         <v>49</v>
       </c>
-      <c r="AD5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="AF5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI5">
-        <v>20190101</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="C6" s="3">
         <v>2018</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F6" t="s">
         <v>5</v>
@@ -1210,13 +1164,13 @@
         <v>29</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="L6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>29</v>
@@ -1257,44 +1211,38 @@
       <c r="Y6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z6" s="3" t="s">
-        <v>61</v>
+      <c r="Z6" s="3">
+        <v>39</v>
       </c>
       <c r="AA6" s="3">
         <v>39</v>
       </c>
-      <c r="AB6" s="3">
-        <v>39</v>
+      <c r="AB6" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="AC6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AE6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AG6">
+        <v>20190101</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>49</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AF6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AG6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AH6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="AI6">
-        <v>20190101</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AK6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL6" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pas-730: range of fixes for daily run
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_CA_CHOICE.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/New2VIN_CA_CHOICE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CSAA\CODE\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732" tabRatio="603"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -558,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AC1" activeCellId="1" sqref="Z1:Z6 AC1:AC6"/>
     </sheetView>
   </sheetViews>

</xml_diff>